<commit_message>
chore: changing some terms
</commit_message>
<xml_diff>
--- a/refs/input2.xlsx
+++ b/refs/input2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Gabriel\Universidade\PO2\refs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11C93357-F8DB-4523-924B-B76C1A291803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE841E4-D076-4119-B0EB-47B47C019B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{A07F0FBE-ABF8-4397-B44B-22BA699F2F5E}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -587,7 +587,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,10 +653,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="4">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="F2" s="4">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="G2" s="4">
         <v>6</v>
@@ -671,7 +671,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="4">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>6</v>
@@ -679,7 +679,7 @@
       <c r="M2" s="4"/>
       <c r="N2" s="6" cm="1">
         <f t="array" ref="N2:N12">MMULT(B2:K12, TRANSPOSE(B13:K13))</f>
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
@@ -813,7 +813,7 @@
         <v>8</v>
       </c>
       <c r="N5" s="7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
@@ -857,7 +857,7 @@
         <v>7</v>
       </c>
       <c r="N6" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
@@ -901,7 +901,7 @@
         <v>6</v>
       </c>
       <c r="N7" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
@@ -945,7 +945,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -1140,10 +1140,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="7">
         <v>0</v>

</xml_diff>